<commit_message>
finish data work flow chart and refactor relative path
</commit_message>
<xml_diff>
--- a/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
+++ b/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
@@ -2371,7 +2371,7 @@
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>In progress</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Withdrawn (SAE)</t>
+          <t>In progress</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
@@ -10874,7 +10874,7 @@
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
-          <t>In progress</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="D160" s="3" t="n">
@@ -10942,8 +10942,16 @@
           <t>05-07-2023</t>
         </is>
       </c>
-      <c r="S160" s="3" t="n"/>
-      <c r="T160" s="3" t="n"/>
+      <c r="S160" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="T160" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="U160" s="3" t="n">
         <v>10</v>
       </c>
@@ -11128,12 +11136,36 @@
           <t>17-07-2023</t>
         </is>
       </c>
-      <c r="N163" s="3" t="n"/>
-      <c r="O163" s="3" t="n"/>
-      <c r="P163" s="3" t="n"/>
-      <c r="Q163" s="3" t="n"/>
-      <c r="R163" s="3" t="n"/>
-      <c r="S163" s="3" t="n"/>
+      <c r="N163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="O163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="P163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="Q163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="R163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="S163" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="T163" s="3" t="n"/>
       <c r="U163" s="3" t="n">
         <v>5</v>
@@ -11261,8 +11293,16 @@
           <t>17-07-2023</t>
         </is>
       </c>
-      <c r="M165" s="3" t="n"/>
-      <c r="N165" s="3" t="n"/>
+      <c r="M165" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="N165" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="O165" s="3" t="n"/>
       <c r="P165" s="3" t="n"/>
       <c r="Q165" s="3" t="n"/>
@@ -11402,8 +11442,16 @@
           <t>21-07-2023</t>
         </is>
       </c>
-      <c r="P167" s="3" t="n"/>
-      <c r="Q167" s="3" t="n"/>
+      <c r="P167" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="Q167" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="R167" s="3" t="n"/>
       <c r="S167" s="3" t="n"/>
       <c r="T167" s="3" t="n"/>
@@ -11465,9 +11513,21 @@
           <t>21-07-2023</t>
         </is>
       </c>
-      <c r="N168" s="3" t="n"/>
-      <c r="O168" s="3" t="n"/>
-      <c r="P168" s="3" t="n"/>
+      <c r="N168" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="O168" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="P168" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="Q168" s="3" t="n"/>
       <c r="R168" s="3" t="n"/>
       <c r="S168" s="3" t="n"/>
@@ -11525,10 +11585,26 @@
           <t>18-07-2023</t>
         </is>
       </c>
-      <c r="M169" s="3" t="n"/>
-      <c r="N169" s="3" t="n"/>
-      <c r="O169" s="3" t="n"/>
-      <c r="P169" s="3" t="n"/>
+      <c r="M169" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="N169" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="O169" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="P169" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="Q169" s="3" t="n"/>
       <c r="R169" s="3" t="n"/>
       <c r="S169" s="3" t="n"/>
@@ -11571,10 +11647,26 @@
           <t>19-07-2023</t>
         </is>
       </c>
-      <c r="J170" s="3" t="n"/>
-      <c r="K170" s="3" t="n"/>
-      <c r="L170" s="3" t="n"/>
-      <c r="M170" s="3" t="n"/>
+      <c r="J170" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="K170" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="L170" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="M170" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="N170" s="3" t="n"/>
       <c r="O170" s="3" t="n"/>
       <c r="P170" s="3" t="n"/>
@@ -11620,10 +11712,26 @@
           <t>20-07-2023</t>
         </is>
       </c>
-      <c r="J171" s="3" t="n"/>
-      <c r="K171" s="3" t="n"/>
-      <c r="L171" s="3" t="n"/>
-      <c r="M171" s="3" t="n"/>
+      <c r="J171" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="K171" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="L171" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="M171" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="N171" s="3" t="n"/>
       <c r="O171" s="3" t="n"/>
       <c r="P171" s="3" t="n"/>
@@ -12816,13 +12924,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
@@ -12873,13 +12981,13 @@
         <v>4</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
@@ -12966,13 +13074,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
@@ -13051,13 +13159,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
@@ -13100,13 +13208,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
@@ -13161,13 +13269,13 @@
         <v>0</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
@@ -13222,13 +13330,13 @@
         <v>4</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
@@ -13510,13 +13618,13 @@
         <v>0</v>
       </c>
       <c r="F27" s="3" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G27" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="3" t="inlineStr">
         <is>
@@ -13577,20 +13685,20 @@
         </is>
       </c>
       <c r="D28" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="G28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F28" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3" t="n">
-        <v>4</v>
-      </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
           <t>12-05-2023</t>
@@ -13613,7 +13721,7 @@
       </c>
       <c r="M28" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>30-06-2023</t>
         </is>
       </c>
       <c r="N28" s="3" t="n"/>
@@ -13624,7 +13732,7 @@
       <c r="S28" s="3" t="n"/>
       <c r="T28" s="3" t="n"/>
       <c r="U28" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -13642,13 +13750,13 @@
         </is>
       </c>
       <c r="D29" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3" t="n">
         <v>21</v>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="F29" s="3" t="n">
-        <v>12</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>0</v>
@@ -13688,36 +13796,36 @@
       </c>
       <c r="O29" s="3" t="inlineStr">
         <is>
+          <t>05-07-2023</t>
+        </is>
+      </c>
+      <c r="P29" s="3" t="inlineStr">
+        <is>
+          <t>15-07-2023</t>
+        </is>
+      </c>
+      <c r="Q29" s="3" t="inlineStr">
+        <is>
           <t>not_match</t>
         </is>
       </c>
-      <c r="P29" s="3" t="inlineStr">
+      <c r="R29" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
         </is>
       </c>
-      <c r="Q29" s="3" t="inlineStr">
+      <c r="S29" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
         </is>
       </c>
-      <c r="R29" s="3" t="inlineStr">
+      <c r="T29" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
         </is>
       </c>
-      <c r="S29" s="3" t="inlineStr">
-        <is>
-          <t>not_match</t>
-        </is>
-      </c>
-      <c r="T29" s="3" t="inlineStr">
-        <is>
-          <t>not_match</t>
-        </is>
-      </c>
       <c r="U29" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -13735,10 +13843,10 @@
         </is>
       </c>
       <c r="D30" s="3" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>12</v>
@@ -13747,7 +13855,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30" s="3" t="inlineStr">
         <is>
@@ -13766,7 +13874,7 @@
       </c>
       <c r="L30" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>30-06-2023</t>
         </is>
       </c>
       <c r="M30" s="3" t="n"/>
@@ -13778,7 +13886,7 @@
       <c r="S30" s="3" t="n"/>
       <c r="T30" s="3" t="n"/>
       <c r="U30" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -13796,20 +13904,20 @@
         </is>
       </c>
       <c r="D31" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="G31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F31" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="G31" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="3" t="n">
-        <v>4</v>
-      </c>
       <c r="I31" s="3" t="inlineStr">
         <is>
           <t>17-05-2023</t>
@@ -13832,7 +13940,7 @@
       </c>
       <c r="M31" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>30-06-2023</t>
         </is>
       </c>
       <c r="N31" s="3" t="n"/>
@@ -13843,7 +13951,7 @@
       <c r="S31" s="3" t="n"/>
       <c r="T31" s="3" t="n"/>
       <c r="U31" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -13861,13 +13969,13 @@
         </is>
       </c>
       <c r="D32" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="n">
         <v>12</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="F32" s="3" t="n">
-        <v>4</v>
       </c>
       <c r="G32" s="3" t="n">
         <v>0</v>
@@ -13892,12 +14000,12 @@
       </c>
       <c r="L32" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>30-06-2023</t>
         </is>
       </c>
       <c r="M32" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>14-07-2023</t>
         </is>
       </c>
       <c r="N32" s="3" t="inlineStr">
@@ -13912,7 +14020,7 @@
       <c r="S32" s="3" t="n"/>
       <c r="T32" s="3" t="n"/>
       <c r="U32" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -13936,13 +14044,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="3" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G33" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I33" s="3" t="inlineStr">
         <is>
@@ -14001,13 +14109,13 @@
         <v>0</v>
       </c>
       <c r="F34" s="3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G34" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I34" s="3" t="inlineStr">
         <is>
@@ -14052,20 +14160,20 @@
         </is>
       </c>
       <c r="D35" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="E35" s="3" t="n">
+      <c r="G35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3" t="n">
-        <v>20</v>
-      </c>
       <c r="I35" s="3" t="inlineStr">
         <is>
           <t>31-05-2023</t>
@@ -14093,12 +14201,12 @@
       </c>
       <c r="N35" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>05-07-2023</t>
         </is>
       </c>
       <c r="O35" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>12-07-2023</t>
         </is>
       </c>
       <c r="P35" s="3" t="inlineStr">
@@ -14115,7 +14223,7 @@
       <c r="S35" s="3" t="n"/>
       <c r="T35" s="3" t="n"/>
       <c r="U35" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -14133,20 +14241,20 @@
         </is>
       </c>
       <c r="D36" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="E36" s="3" t="n">
+      <c r="G36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="3" t="n">
-        <v>16</v>
-      </c>
       <c r="I36" s="3" t="inlineStr">
         <is>
           <t>07-06-2023</t>
@@ -14169,12 +14277,12 @@
       </c>
       <c r="M36" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>05-07-2023</t>
         </is>
       </c>
       <c r="N36" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>12-07-2023</t>
         </is>
       </c>
       <c r="O36" s="3" t="inlineStr">
@@ -14200,7 +14308,7 @@
       <c r="S36" s="3" t="n"/>
       <c r="T36" s="3" t="n"/>
       <c r="U36" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -14224,13 +14332,13 @@
         <v>0</v>
       </c>
       <c r="F37" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G37" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I37" s="3" t="inlineStr">
         <is>
@@ -14271,19 +14379,19 @@
         </is>
       </c>
       <c r="D38" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E38" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E38" s="3" t="n">
-        <v>12</v>
-      </c>
       <c r="F38" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G38" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I38" s="3" t="inlineStr">
         <is>
@@ -14297,12 +14405,12 @@
       </c>
       <c r="K38" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>10-07-2023</t>
         </is>
       </c>
       <c r="L38" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>17-07-2023</t>
         </is>
       </c>
       <c r="M38" s="3" t="inlineStr">
@@ -14334,7 +14442,7 @@
       <c r="S38" s="3" t="n"/>
       <c r="T38" s="3" t="n"/>
       <c r="U38" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -14358,13 +14466,13 @@
         <v>0</v>
       </c>
       <c r="F39" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G39" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I39" s="3" t="inlineStr">
         <is>
@@ -14404,24 +14512,34 @@
           <t>In progress</t>
         </is>
       </c>
-      <c r="D40" s="3" t="n"/>
-      <c r="E40" s="3" t="n"/>
-      <c r="F40" s="3" t="n"/>
-      <c r="G40" s="3" t="n"/>
-      <c r="H40" s="3" t="n"/>
+      <c r="D40" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="I40" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>05-07-2023</t>
         </is>
       </c>
       <c r="J40" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>12-07-2023</t>
         </is>
       </c>
       <c r="K40" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>19-07-2023</t>
         </is>
       </c>
       <c r="L40" s="3" t="inlineStr">
@@ -14449,7 +14567,9 @@
       <c r="R40" s="3" t="n"/>
       <c r="S40" s="3" t="n"/>
       <c r="T40" s="3" t="n"/>
-      <c r="U40" s="3" t="n"/>
+      <c r="U40" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
@@ -14472,13 +14592,13 @@
         <v>0</v>
       </c>
       <c r="F41" s="3" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G41" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I41" s="3" t="inlineStr">
         <is>
@@ -14525,13 +14645,13 @@
         <v>0</v>
       </c>
       <c r="F42" s="3" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G42" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I42" s="3" t="inlineStr">
         <is>
@@ -14590,13 +14710,13 @@
         <v>0</v>
       </c>
       <c r="F43" s="3" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G43" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="3" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="I43" s="3" t="inlineStr">
         <is>
@@ -14651,13 +14771,13 @@
         <v>0</v>
       </c>
       <c r="F44" s="3" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G44" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="3" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3" t="inlineStr">
         <is>
@@ -14720,13 +14840,13 @@
         <v>0</v>
       </c>
       <c r="F45" s="3" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G45" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H45" s="3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I45" s="3" t="inlineStr">
         <is>
@@ -14813,13 +14933,13 @@
         <v>0</v>
       </c>
       <c r="F46" s="3" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G46" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="3" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I46" s="3" t="inlineStr">
         <is>
@@ -14878,13 +14998,13 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G47" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I47" s="3" t="inlineStr">
         <is>
@@ -14935,13 +15055,13 @@
         <v>0</v>
       </c>
       <c r="F48" s="3" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G48" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I48" s="3" t="inlineStr">
         <is>
@@ -15221,19 +15341,19 @@
         </is>
       </c>
       <c r="D52" s="3" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F52" s="3" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G52" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H52" s="3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I52" s="3" t="inlineStr">
         <is>
@@ -15247,12 +15367,12 @@
       </c>
       <c r="K52" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>19-07-2023</t>
         </is>
       </c>
       <c r="L52" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>11-08-2023</t>
         </is>
       </c>
       <c r="M52" s="3" t="inlineStr">
@@ -15268,7 +15388,7 @@
       <c r="S52" s="3" t="n"/>
       <c r="T52" s="3" t="n"/>
       <c r="U52" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -15286,19 +15406,19 @@
         </is>
       </c>
       <c r="D53" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F53" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E53" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="F53" s="3" t="n">
-        <v>0</v>
-      </c>
       <c r="G53" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I53" s="3" t="inlineStr">
         <is>
@@ -15312,7 +15432,7 @@
       </c>
       <c r="K53" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>22-08-2023</t>
         </is>
       </c>
       <c r="L53" s="3" t="n"/>
@@ -15325,7 +15445,7 @@
       <c r="S53" s="3" t="n"/>
       <c r="T53" s="3" t="n"/>
       <c r="U53" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -15342,11 +15462,21 @@
           <t xml:space="preserve">Completed </t>
         </is>
       </c>
-      <c r="D54" s="3" t="n"/>
-      <c r="E54" s="3" t="n"/>
-      <c r="F54" s="3" t="n"/>
-      <c r="G54" s="3" t="n"/>
-      <c r="H54" s="3" t="n"/>
+      <c r="D54" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="I54" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
@@ -15354,7 +15484,7 @@
       </c>
       <c r="J54" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>19-07-2023</t>
         </is>
       </c>
       <c r="K54" s="3" t="n"/>
@@ -15367,7 +15497,9 @@
       <c r="R54" s="3" t="n"/>
       <c r="S54" s="3" t="n"/>
       <c r="T54" s="3" t="n"/>
-      <c r="U54" s="3" t="n"/>
+      <c r="U54" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
@@ -15383,11 +15515,21 @@
           <t>In progress</t>
         </is>
       </c>
-      <c r="D55" s="3" t="n"/>
-      <c r="E55" s="3" t="n"/>
-      <c r="F55" s="3" t="n"/>
-      <c r="G55" s="3" t="n"/>
-      <c r="H55" s="3" t="n"/>
+      <c r="D55" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="I55" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
@@ -15395,12 +15537,12 @@
       </c>
       <c r="J55" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>19-07-2023</t>
         </is>
       </c>
       <c r="K55" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>04-08-2023</t>
         </is>
       </c>
       <c r="L55" s="3" t="n"/>
@@ -15412,7 +15554,9 @@
       <c r="R55" s="3" t="n"/>
       <c r="S55" s="3" t="n"/>
       <c r="T55" s="3" t="n"/>
-      <c r="U55" s="3" t="n"/>
+      <c r="U55" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
@@ -15428,11 +15572,21 @@
           <t>Withdrawn (SAE)</t>
         </is>
       </c>
-      <c r="D56" s="3" t="n"/>
-      <c r="E56" s="3" t="n"/>
-      <c r="F56" s="3" t="n"/>
-      <c r="G56" s="3" t="n"/>
-      <c r="H56" s="3" t="n"/>
+      <c r="D56" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>2</v>
+      </c>
       <c r="I56" s="3" t="inlineStr">
         <is>
           <t>not_match</t>
@@ -15440,7 +15594,7 @@
       </c>
       <c r="J56" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="K56" s="3" t="n"/>
@@ -15453,7 +15607,9 @@
       <c r="R56" s="3" t="n"/>
       <c r="S56" s="3" t="n"/>
       <c r="T56" s="3" t="n"/>
-      <c r="U56" s="3" t="n"/>
+      <c r="U56" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
@@ -15872,13 +16028,13 @@
         <v>0</v>
       </c>
       <c r="F65" s="3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G65" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H65" s="3" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I65" s="3" t="inlineStr">
         <is>
@@ -16029,19 +16185,19 @@
         </is>
       </c>
       <c r="D68" s="3" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G68" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H68" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I68" s="3" t="inlineStr">
         <is>
@@ -16050,7 +16206,7 @@
       </c>
       <c r="J68" s="3" t="inlineStr">
         <is>
-          <t>not_match</t>
+          <t>11-08-2023</t>
         </is>
       </c>
       <c r="K68" s="3" t="inlineStr">
@@ -16068,7 +16224,7 @@
       <c r="S68" s="3" t="n"/>
       <c r="T68" s="3" t="n"/>
       <c r="U68" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">

</xml_diff>

<commit_message>
optimize dfu match and summary function
</commit_message>
<xml_diff>
--- a/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
+++ b/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>506</v>
+        <v>690</v>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>4644</v>
+        <v>4828</v>
       </c>
       <c r="D8" s="3" t="n"/>
     </row>
@@ -610,7 +610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U171"/>
+  <dimension ref="A1:U176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5364,14 +5364,36 @@
       <c r="B68" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C68" s="3" t="n"/>
-      <c r="D68" s="3" t="n"/>
-      <c r="E68" s="3" t="n"/>
-      <c r="F68" s="3" t="n"/>
-      <c r="G68" s="3" t="n"/>
-      <c r="H68" s="3" t="n"/>
-      <c r="I68" s="3" t="n"/>
-      <c r="J68" s="3" t="n"/>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="K68" s="3" t="n"/>
       <c r="L68" s="3" t="n"/>
       <c r="M68" s="3" t="n"/>
@@ -5382,7 +5404,9 @@
       <c r="R68" s="3" t="n"/>
       <c r="S68" s="3" t="n"/>
       <c r="T68" s="3" t="n"/>
-      <c r="U68" s="3" t="n"/>
+      <c r="U68" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
@@ -5393,15 +5417,41 @@
       <c r="B69" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C69" s="3" t="n"/>
-      <c r="D69" s="3" t="n"/>
-      <c r="E69" s="3" t="n"/>
-      <c r="F69" s="3" t="n"/>
-      <c r="G69" s="3" t="n"/>
-      <c r="H69" s="3" t="n"/>
-      <c r="I69" s="3" t="n"/>
-      <c r="J69" s="3" t="n"/>
-      <c r="K69" s="3" t="n"/>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>30-08-2023</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="L69" s="3" t="n"/>
       <c r="M69" s="3" t="n"/>
       <c r="N69" s="3" t="n"/>
@@ -5411,7 +5461,9 @@
       <c r="R69" s="3" t="n"/>
       <c r="S69" s="3" t="n"/>
       <c r="T69" s="3" t="n"/>
-      <c r="U69" s="3" t="n"/>
+      <c r="U69" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
@@ -5422,13 +5474,31 @@
       <c r="B70" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C70" s="3" t="n"/>
-      <c r="D70" s="3" t="n"/>
-      <c r="E70" s="3" t="n"/>
-      <c r="F70" s="3" t="n"/>
-      <c r="G70" s="3" t="n"/>
-      <c r="H70" s="3" t="n"/>
-      <c r="I70" s="3" t="n"/>
+      <c r="C70" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
       <c r="J70" s="3" t="n"/>
       <c r="K70" s="3" t="n"/>
       <c r="L70" s="3" t="n"/>
@@ -5440,7 +5510,9 @@
       <c r="R70" s="3" t="n"/>
       <c r="S70" s="3" t="n"/>
       <c r="T70" s="3" t="n"/>
-      <c r="U70" s="3" t="n"/>
+      <c r="U70" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
@@ -5451,15 +5523,41 @@
       <c r="B71" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C71" s="3" t="n"/>
-      <c r="D71" s="3" t="n"/>
-      <c r="E71" s="3" t="n"/>
-      <c r="F71" s="3" t="n"/>
-      <c r="G71" s="3" t="n"/>
-      <c r="H71" s="3" t="n"/>
-      <c r="I71" s="3" t="n"/>
-      <c r="J71" s="3" t="n"/>
-      <c r="K71" s="3" t="n"/>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I71" s="3" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="K71" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="L71" s="3" t="n"/>
       <c r="M71" s="3" t="n"/>
       <c r="N71" s="3" t="n"/>
@@ -5469,7 +5567,9 @@
       <c r="R71" s="3" t="n"/>
       <c r="S71" s="3" t="n"/>
       <c r="T71" s="3" t="n"/>
-      <c r="U71" s="3" t="n"/>
+      <c r="U71" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
@@ -5480,13 +5580,31 @@
       <c r="B72" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C72" s="3" t="n"/>
-      <c r="D72" s="3" t="n"/>
-      <c r="E72" s="3" t="n"/>
-      <c r="F72" s="3" t="n"/>
-      <c r="G72" s="3" t="n"/>
-      <c r="H72" s="3" t="n"/>
-      <c r="I72" s="3" t="n"/>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I72" s="3" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
       <c r="J72" s="3" t="n"/>
       <c r="K72" s="3" t="n"/>
       <c r="L72" s="3" t="n"/>
@@ -5498,7 +5616,9 @@
       <c r="R72" s="3" t="n"/>
       <c r="S72" s="3" t="n"/>
       <c r="T72" s="3" t="n"/>
-      <c r="U72" s="3" t="n"/>
+      <c r="U72" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
@@ -9989,9 +10109,21 @@
           <t>21-08-2023</t>
         </is>
       </c>
-      <c r="N144" s="3" t="n"/>
-      <c r="O144" s="3" t="n"/>
-      <c r="P144" s="3" t="n"/>
+      <c r="N144" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="O144" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="P144" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="Q144" s="3" t="n"/>
       <c r="R144" s="3" t="n"/>
       <c r="S144" s="3" t="n"/>
@@ -10044,9 +10176,21 @@
           <t>21-08-2023</t>
         </is>
       </c>
-      <c r="L145" s="3" t="n"/>
-      <c r="M145" s="3" t="n"/>
-      <c r="N145" s="3" t="n"/>
+      <c r="L145" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="M145" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="N145" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="O145" s="3" t="n"/>
       <c r="P145" s="3" t="n"/>
       <c r="Q145" s="3" t="n"/>
@@ -10150,9 +10294,21 @@
           <t>15-08-2023</t>
         </is>
       </c>
-      <c r="L147" s="3" t="n"/>
-      <c r="M147" s="3" t="n"/>
-      <c r="N147" s="3" t="n"/>
+      <c r="L147" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="M147" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="N147" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="O147" s="3" t="n"/>
       <c r="P147" s="3" t="n"/>
       <c r="Q147" s="3" t="n"/>
@@ -10197,9 +10353,21 @@
           <t>15-08-2023</t>
         </is>
       </c>
-      <c r="J148" s="3" t="n"/>
-      <c r="K148" s="3" t="n"/>
-      <c r="L148" s="3" t="n"/>
+      <c r="J148" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="K148" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="L148" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="M148" s="3" t="n"/>
       <c r="N148" s="3" t="n"/>
       <c r="O148" s="3" t="n"/>
@@ -10241,9 +10409,21 @@
           <t>not match</t>
         </is>
       </c>
-      <c r="K149" s="3" t="n"/>
-      <c r="L149" s="3" t="n"/>
-      <c r="M149" s="3" t="n"/>
+      <c r="K149" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="L149" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="M149" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="N149" s="3" t="n"/>
       <c r="O149" s="3" t="n"/>
       <c r="P149" s="3" t="n"/>
@@ -10287,7 +10467,11 @@
           <t>16-08-2023</t>
         </is>
       </c>
-      <c r="J150" s="3" t="n"/>
+      <c r="J150" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
       <c r="K150" s="3" t="n"/>
       <c r="L150" s="3" t="n"/>
       <c r="M150" s="3" t="n"/>
@@ -10870,7 +11054,7 @@
         </is>
       </c>
       <c r="B160" s="3" t="n">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C160" s="3" t="inlineStr">
         <is>
@@ -10878,7 +11062,7 @@
         </is>
       </c>
       <c r="D160" s="3" t="n">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E160" s="3" t="n">
         <v>0</v>
@@ -10890,7 +11074,7 @@
         <v>11</v>
       </c>
       <c r="H160" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I160" s="3" t="inlineStr">
         <is>
@@ -10944,16 +11128,16 @@
       </c>
       <c r="S160" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>03-08-2023</t>
         </is>
       </c>
       <c r="T160" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>15-08-2023</t>
         </is>
       </c>
       <c r="U160" s="3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161">
@@ -11089,7 +11273,7 @@
         </is>
       </c>
       <c r="B163" s="3" t="n">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C163" s="3" t="inlineStr">
         <is>
@@ -11097,10 +11281,10 @@
         </is>
       </c>
       <c r="D163" s="3" t="n">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F163" s="3" t="n">
         <v>25</v>
@@ -11109,7 +11293,7 @@
         <v>6</v>
       </c>
       <c r="H163" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I163" s="3" t="inlineStr">
         <is>
@@ -11138,37 +11322,37 @@
       </c>
       <c r="N163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>01-08-2023</t>
         </is>
       </c>
       <c r="O163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>08-08-2023</t>
         </is>
       </c>
       <c r="P163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>15-08-2023</t>
         </is>
       </c>
       <c r="Q163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>22-08-2023</t>
         </is>
       </c>
       <c r="R163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>29-08-2023</t>
         </is>
       </c>
       <c r="S163" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>05-09-2023</t>
         </is>
       </c>
       <c r="T163" s="3" t="n"/>
       <c r="U163" s="3" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164">
@@ -11251,7 +11435,7 @@
         </is>
       </c>
       <c r="B165" s="3" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C165" s="3" t="inlineStr">
         <is>
@@ -11259,7 +11443,7 @@
         </is>
       </c>
       <c r="D165" s="3" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E165" s="3" t="n">
         <v>0</v>
@@ -11271,7 +11455,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="3" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I165" s="3" t="inlineStr">
         <is>
@@ -11295,12 +11479,12 @@
       </c>
       <c r="M165" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>27-07-2023</t>
         </is>
       </c>
       <c r="N165" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>10-08-2023</t>
         </is>
       </c>
       <c r="O165" s="3" t="n"/>
@@ -11310,7 +11494,7 @@
       <c r="S165" s="3" t="n"/>
       <c r="T165" s="3" t="n"/>
       <c r="U165" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166">
@@ -11385,7 +11569,7 @@
         </is>
       </c>
       <c r="B167" s="3" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C167" s="3" t="inlineStr">
         <is>
@@ -11393,7 +11577,7 @@
         </is>
       </c>
       <c r="D167" s="3" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E167" s="3" t="n">
         <v>0</v>
@@ -11405,7 +11589,7 @@
         <v>0</v>
       </c>
       <c r="H167" s="3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I167" s="3" t="inlineStr">
         <is>
@@ -11444,19 +11628,19 @@
       </c>
       <c r="P167" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>30-08-2023</t>
         </is>
       </c>
       <c r="Q167" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>05-09-2023</t>
         </is>
       </c>
       <c r="R167" s="3" t="n"/>
       <c r="S167" s="3" t="n"/>
       <c r="T167" s="3" t="n"/>
       <c r="U167" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168">
@@ -11466,7 +11650,7 @@
         </is>
       </c>
       <c r="B168" s="3" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C168" s="3" t="inlineStr">
         <is>
@@ -11474,7 +11658,7 @@
         </is>
       </c>
       <c r="D168" s="3" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E168" s="3" t="n">
         <v>0</v>
@@ -11486,7 +11670,7 @@
         <v>0</v>
       </c>
       <c r="H168" s="3" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I168" s="3" t="inlineStr">
         <is>
@@ -11515,17 +11699,17 @@
       </c>
       <c r="N168" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>27-07-2023</t>
         </is>
       </c>
       <c r="O168" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>03-08-2023</t>
         </is>
       </c>
       <c r="P168" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>14-08-2023</t>
         </is>
       </c>
       <c r="Q168" s="3" t="n"/>
@@ -11533,7 +11717,7 @@
       <c r="S168" s="3" t="n"/>
       <c r="T168" s="3" t="n"/>
       <c r="U168" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169">
@@ -11543,7 +11727,7 @@
         </is>
       </c>
       <c r="B169" s="3" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C169" s="3" t="inlineStr">
         <is>
@@ -11551,7 +11735,7 @@
         </is>
       </c>
       <c r="D169" s="3" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E169" s="3" t="n">
         <v>0</v>
@@ -11563,7 +11747,7 @@
         <v>0</v>
       </c>
       <c r="H169" s="3" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I169" s="3" t="inlineStr">
         <is>
@@ -11587,22 +11771,22 @@
       </c>
       <c r="M169" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>31-07-2023</t>
         </is>
       </c>
       <c r="N169" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>08-08-2023</t>
         </is>
       </c>
       <c r="O169" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>21-08-2023</t>
         </is>
       </c>
       <c r="P169" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>04-09-2023</t>
         </is>
       </c>
       <c r="Q169" s="3" t="n"/>
@@ -11610,7 +11794,7 @@
       <c r="S169" s="3" t="n"/>
       <c r="T169" s="3" t="n"/>
       <c r="U169" s="3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="170">
@@ -11620,7 +11804,7 @@
         </is>
       </c>
       <c r="B170" s="3" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C170" s="3" t="inlineStr">
         <is>
@@ -11628,7 +11812,7 @@
         </is>
       </c>
       <c r="D170" s="3" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E170" s="3" t="n">
         <v>0</v>
@@ -11640,7 +11824,7 @@
         <v>0</v>
       </c>
       <c r="H170" s="3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I170" s="3" t="inlineStr">
         <is>
@@ -11649,22 +11833,22 @@
       </c>
       <c r="J170" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>26-07-2023</t>
         </is>
       </c>
       <c r="K170" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>02-08-2023</t>
         </is>
       </c>
       <c r="L170" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>16-08-2023</t>
         </is>
       </c>
       <c r="M170" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>28-08-2023</t>
         </is>
       </c>
       <c r="N170" s="3" t="n"/>
@@ -11675,7 +11859,7 @@
       <c r="S170" s="3" t="n"/>
       <c r="T170" s="3" t="n"/>
       <c r="U170" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171">
@@ -11685,7 +11869,7 @@
         </is>
       </c>
       <c r="B171" s="3" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C171" s="3" t="inlineStr">
         <is>
@@ -11693,7 +11877,7 @@
         </is>
       </c>
       <c r="D171" s="3" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E171" s="3" t="n">
         <v>0</v>
@@ -11705,7 +11889,7 @@
         <v>0</v>
       </c>
       <c r="H171" s="3" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I171" s="3" t="inlineStr">
         <is>
@@ -11714,22 +11898,22 @@
       </c>
       <c r="J171" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>27-07-2023</t>
         </is>
       </c>
       <c r="K171" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>10-08-2023</t>
         </is>
       </c>
       <c r="L171" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>18-08-2023</t>
         </is>
       </c>
       <c r="M171" s="3" t="inlineStr">
         <is>
-          <t>not match</t>
+          <t>04-09-2023</t>
         </is>
       </c>
       <c r="N171" s="3" t="n"/>
@@ -11740,6 +11924,243 @@
       <c r="S171" s="3" t="n"/>
       <c r="T171" s="3" t="n"/>
       <c r="U171" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="3" t="inlineStr">
+        <is>
+          <t>292-016</t>
+        </is>
+      </c>
+      <c r="B172" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C172" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D172" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H172" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I172" s="3" t="inlineStr">
+        <is>
+          <t>03-08-2023</t>
+        </is>
+      </c>
+      <c r="J172" s="3" t="inlineStr">
+        <is>
+          <t>09-08-2023</t>
+        </is>
+      </c>
+      <c r="K172" s="3" t="n"/>
+      <c r="L172" s="3" t="n"/>
+      <c r="M172" s="3" t="n"/>
+      <c r="N172" s="3" t="n"/>
+      <c r="O172" s="3" t="n"/>
+      <c r="P172" s="3" t="n"/>
+      <c r="Q172" s="3" t="n"/>
+      <c r="R172" s="3" t="n"/>
+      <c r="S172" s="3" t="n"/>
+      <c r="T172" s="3" t="n"/>
+      <c r="U172" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="3" t="inlineStr">
+        <is>
+          <t>292-017</t>
+        </is>
+      </c>
+      <c r="B173" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C173" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D173" s="3" t="n"/>
+      <c r="E173" s="3" t="n"/>
+      <c r="F173" s="3" t="n"/>
+      <c r="G173" s="3" t="n"/>
+      <c r="H173" s="3" t="n"/>
+      <c r="I173" s="3" t="inlineStr">
+        <is>
+          <t>not match</t>
+        </is>
+      </c>
+      <c r="J173" s="3" t="n"/>
+      <c r="K173" s="3" t="n"/>
+      <c r="L173" s="3" t="n"/>
+      <c r="M173" s="3" t="n"/>
+      <c r="N173" s="3" t="n"/>
+      <c r="O173" s="3" t="n"/>
+      <c r="P173" s="3" t="n"/>
+      <c r="Q173" s="3" t="n"/>
+      <c r="R173" s="3" t="n"/>
+      <c r="S173" s="3" t="n"/>
+      <c r="T173" s="3" t="n"/>
+      <c r="U173" s="3" t="n"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="3" t="inlineStr">
+        <is>
+          <t>292-018</t>
+        </is>
+      </c>
+      <c r="B174" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C174" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D174" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E174" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G174" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="I174" s="3" t="inlineStr">
+        <is>
+          <t>06-09-2023</t>
+        </is>
+      </c>
+      <c r="J174" s="3" t="n"/>
+      <c r="K174" s="3" t="n"/>
+      <c r="L174" s="3" t="n"/>
+      <c r="M174" s="3" t="n"/>
+      <c r="N174" s="3" t="n"/>
+      <c r="O174" s="3" t="n"/>
+      <c r="P174" s="3" t="n"/>
+      <c r="Q174" s="3" t="n"/>
+      <c r="R174" s="3" t="n"/>
+      <c r="S174" s="3" t="n"/>
+      <c r="T174" s="3" t="n"/>
+      <c r="U174" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="3" t="inlineStr">
+        <is>
+          <t>292-019</t>
+        </is>
+      </c>
+      <c r="B175" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C175" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D175" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E175" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G175" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H175" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I175" s="3" t="inlineStr">
+        <is>
+          <t>07-09-2023</t>
+        </is>
+      </c>
+      <c r="J175" s="3" t="n"/>
+      <c r="K175" s="3" t="n"/>
+      <c r="L175" s="3" t="n"/>
+      <c r="M175" s="3" t="n"/>
+      <c r="N175" s="3" t="n"/>
+      <c r="O175" s="3" t="n"/>
+      <c r="P175" s="3" t="n"/>
+      <c r="Q175" s="3" t="n"/>
+      <c r="R175" s="3" t="n"/>
+      <c r="S175" s="3" t="n"/>
+      <c r="T175" s="3" t="n"/>
+      <c r="U175" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="3" t="inlineStr">
+        <is>
+          <t>292-020</t>
+        </is>
+      </c>
+      <c r="B176" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C176" s="3" t="inlineStr">
+        <is>
+          <t>In progress</t>
+        </is>
+      </c>
+      <c r="D176" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E176" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G176" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H176" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I176" s="3" t="inlineStr">
+        <is>
+          <t>07-09-2023</t>
+        </is>
+      </c>
+      <c r="J176" s="3" t="n"/>
+      <c r="K176" s="3" t="n"/>
+      <c r="L176" s="3" t="n"/>
+      <c r="M176" s="3" t="n"/>
+      <c r="N176" s="3" t="n"/>
+      <c r="O176" s="3" t="n"/>
+      <c r="P176" s="3" t="n"/>
+      <c r="Q176" s="3" t="n"/>
+      <c r="R176" s="3" t="n"/>
+      <c r="S176" s="3" t="n"/>
+      <c r="T176" s="3" t="n"/>
+      <c r="U176" s="3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade dfu data organization function
</commit_message>
<xml_diff>
--- a/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
+++ b/Documents/DFU_Summary/WAUSI_Summary_Calculation.xlsx
@@ -2077,7 +2077,7 @@
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Withdrawn</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Withdrawn (SAE)</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Withdrawn</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">

</xml_diff>